<commit_message>
Merged Jamie's code into Master
</commit_message>
<xml_diff>
--- a/Lab 1/Data/data_description.xlsx
+++ b/Lab 1/Data/data_description.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walt\Desktop\datascience\7331\ML1-Visualization-and-Data-Preprocessing-jamie_proj1\ML1-Visualization-and-Data-Preprocessing-jamie_proj1\Lab 1\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Attributes</t>
   </si>
@@ -97,85 +92,13 @@
   </si>
   <si>
     <t>Record Source</t>
-  </si>
-  <si>
-    <t>Unique record identifier generated by MAP based upon the YEAR, MONTH, INCIDENT and ORI code in the report. Alphanumeric 16-character format (A16).</t>
-  </si>
-  <si>
-    <t>The alphanumeric variable describing the name of the law enforcement agency making the report. (A450).</t>
-  </si>
-  <si>
-    <t>– The one-digit numeric code describing the type of law enforcement agency making the report so that 1=Sheriff, 2=County Police, 3=Municipality, 5=Primary State Law Enforcement usually meaning the State Police, 6=Special Police, 7=Constable, 8=Tribal Police, 9=Regional Police. When using the Comma Separated Values format file (file extension=.csv) the original FBI numbering scheme is replaced with the alphanumeric label. (F1.0).</t>
-  </si>
-  <si>
-    <t>Alphanumeric variable describing the original FBI naming and abbreviating scheme for the state of the reporting agency. (A6).</t>
-  </si>
-  <si>
-    <t>The one-digit numeric code describing the type of law enforcement agency making the report so that 1=Sheriff, 2=County Police, 3=Municipality, 5=Primary State Law Enforcement usually meaning the State Police, 6=Special Police, 7=Constable, 8=Tribal Police, 9=Regional Police. When using the Comma Separated Values format file (file extension=.csv) the original FBI numbering scheme is replaced with the alphanumeric label. (F1.0).</t>
-  </si>
-  <si>
-    <t>Year of homicide (or when victim’s body was recovered.) Numeric four digit. (F4.0).</t>
-  </si>
-  <si>
-    <t>– A three-digit number describing the case number within the month in which a homicide occurred. This does not necessarily correspond to the actual case number used inhouse by police agencies. It is used to assist in building a unique record number for each case and to differentiate each case reported within the same month. (F3.0)</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable defining whether the report was “A” = “Murder or Nonnegligent manslaughter” or “B” = “Manslaughter by Negligence.” (A1).</t>
-  </si>
-  <si>
-    <t>MAP-generated indicator whether Offender was identified at time report was made (SOLVED=1) or not identified (SOLVED=0). Numeric single digit format. (F1.0).</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable representing whether the victim was “M” = ”Male” or “F” = ”Female” or “U” indicating “Unknown” gender, usually for conditions in which incomplete remains were recovered. (A1).</t>
-  </si>
-  <si>
-    <t>A three-digit numeric variable describing the age in years of the victim. To allow for simpler mathematical calculations, MAP has changed the original alphanumeric coding of “NB” for new born and “BB” for infant to a numeric value of zero to indicate the victim had not achieved a full year of life. A value of 99, as in the original numbering scheme, represents all victims 99 or older. A value of 999 represents victims whose age was not reported, usually because the victim was unidentified and the age was unknown. (F3.0).</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable representing whether the victim was “A” = “Asian or Pacific Islander” or “B” = “Black” or “I” = “American Indian or Alaskan Native” or “W” = “White” or “U” victim was of “Unknown” race. (A1).</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable representing whether the victim was “H” = “Hispanic Origin” or “N” = “Not of Hispanic Origin” or “U” = “Unknown or Not Reported.” It should be noted that many agencies decline reporting the ethnicity of victims and offenders. (A1).</t>
-  </si>
-  <si>
-    <t>– An alphanumeric variable representing whether the offender was “M”=”Male” or “F”=”Female” or “U” indicating “Unknown” gender, usually in conditions in which the offender had not been identified at the time of the report. (A1).</t>
-  </si>
-  <si>
-    <t>A three-digit numeric variable describing the age in years of the offender. When the offender was not identified at the time of the report, age was reported as 999. A value of 99 represents all offenders 99 or older. (F3.0).</t>
-  </si>
-  <si>
-    <t>– An alphanumeric variable representing whether the offender was “A” = “Asian or Pacific Islander” or “B” = “Black” or “I” = “American Indian or Alaskan Native” or “W” = “White” or “U” = “Unknown” race, usually in conditions in which the offender had not been identified at the time of the report. (A1).</t>
-  </si>
-  <si>
-    <t>– An alphanumeric variable representing whether the offender was “H” = “Hispanic Origin” or “N” = “Not of Hispanic Origin” or “U” = “Unknown or Not Reported.” It should be noted that many agencies decline reporting the ethnicity of victims and offenders. (A1).</t>
-  </si>
-  <si>
-    <t>– A two-digit numeric variable representing the weapon used in the crime. (F2.0).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An alphanumeric variable describing the relationship between the victim and the offender, if any. </t>
-  </si>
-  <si>
-    <t>The number of additional victims (not counting the victim included in the current record) included in the Supplementary Homicide Report’s incident record, which can accept up to 10 additional victims in a single incident report. (F3.0) Incidents of mass murder of more than 11 victims would require multiple SHR incident reports. The Murder Accountability Project’s database captures all reported homicide victims as separate cases. Associated victims will have identical ID numbers</t>
-  </si>
-  <si>
-    <t>The number of additional offenders (not counting the offender included in the current record) included in the Supplementary Homicide Report’s incident record, which can accept up to 10 additional offenders in a single incident report. (F3.0) Unlike victims, the Murder Accountability Project does not create multiple case reports for additional offenders. Only the first offender listed in the original SHR report is included.</t>
-  </si>
-  <si>
-    <t>An eight-digit numeric variable representing the Census Bureau’s Federal Information Processing Standards (FIPS) code for the Metropolitan Statistical Area from which a record was reported. When using the Comma Separated Values format file (file extension=.csv) the original FIPS coding is replaced with the label indicating the metropolitan area. (F8.0).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The month of homicide occurrence or when the victim’s body was recovered. </t>
-  </si>
-  <si>
-    <t>MAP-generated identifier if record provided by FBI (SOURCE=1) or was obtained by MAP under the Freedom of Information Act from an Agency not participating in SHR reporting to the FBI (SOURCE=0). Numeric single digit format. (F1.0).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,13 +150,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -241,14 +161,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -295,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -327,27 +239,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,24 +273,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -572,16 +448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -589,268 +463,196 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="210" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Resolved compile issue for Time Series plot
</commit_message>
<xml_diff>
--- a/Lab 1/Data/data_description.xlsx
+++ b/Lab 1/Data/data_description.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walt\Desktop\datascience\7331\ML1-Visualization-and-Data-Preprocessing-jamie_proj1\ML1-Visualization-and-Data-Preprocessing-jamie_proj1\Lab 1\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Attributes</t>
   </si>
@@ -92,13 +97,85 @@
   </si>
   <si>
     <t>Record Source</t>
+  </si>
+  <si>
+    <t>Unique record identifier generated by MAP based upon the YEAR, MONTH, INCIDENT and ORI code in the report. Alphanumeric 16-character format (A16).</t>
+  </si>
+  <si>
+    <t>The alphanumeric variable describing the name of the law enforcement agency making the report. (A450).</t>
+  </si>
+  <si>
+    <t>– The one-digit numeric code describing the type of law enforcement agency making the report so that 1=Sheriff, 2=County Police, 3=Municipality, 5=Primary State Law Enforcement usually meaning the State Police, 6=Special Police, 7=Constable, 8=Tribal Police, 9=Regional Police. When using the Comma Separated Values format file (file extension=.csv) the original FBI numbering scheme is replaced with the alphanumeric label. (F1.0).</t>
+  </si>
+  <si>
+    <t>Alphanumeric variable describing the original FBI naming and abbreviating scheme for the state of the reporting agency. (A6).</t>
+  </si>
+  <si>
+    <t>The one-digit numeric code describing the type of law enforcement agency making the report so that 1=Sheriff, 2=County Police, 3=Municipality, 5=Primary State Law Enforcement usually meaning the State Police, 6=Special Police, 7=Constable, 8=Tribal Police, 9=Regional Police. When using the Comma Separated Values format file (file extension=.csv) the original FBI numbering scheme is replaced with the alphanumeric label. (F1.0).</t>
+  </si>
+  <si>
+    <t>Year of homicide (or when victim’s body was recovered.) Numeric four digit. (F4.0).</t>
+  </si>
+  <si>
+    <t>– A three-digit number describing the case number within the month in which a homicide occurred. This does not necessarily correspond to the actual case number used inhouse by police agencies. It is used to assist in building a unique record number for each case and to differentiate each case reported within the same month. (F3.0)</t>
+  </si>
+  <si>
+    <t>An alphanumeric variable defining whether the report was “A” = “Murder or Nonnegligent manslaughter” or “B” = “Manslaughter by Negligence.” (A1).</t>
+  </si>
+  <si>
+    <t>MAP-generated indicator whether Offender was identified at time report was made (SOLVED=1) or not identified (SOLVED=0). Numeric single digit format. (F1.0).</t>
+  </si>
+  <si>
+    <t>An alphanumeric variable representing whether the victim was “M” = ”Male” or “F” = ”Female” or “U” indicating “Unknown” gender, usually for conditions in which incomplete remains were recovered. (A1).</t>
+  </si>
+  <si>
+    <t>A three-digit numeric variable describing the age in years of the victim. To allow for simpler mathematical calculations, MAP has changed the original alphanumeric coding of “NB” for new born and “BB” for infant to a numeric value of zero to indicate the victim had not achieved a full year of life. A value of 99, as in the original numbering scheme, represents all victims 99 or older. A value of 999 represents victims whose age was not reported, usually because the victim was unidentified and the age was unknown. (F3.0).</t>
+  </si>
+  <si>
+    <t>An alphanumeric variable representing whether the victim was “A” = “Asian or Pacific Islander” or “B” = “Black” or “I” = “American Indian or Alaskan Native” or “W” = “White” or “U” victim was of “Unknown” race. (A1).</t>
+  </si>
+  <si>
+    <t>An alphanumeric variable representing whether the victim was “H” = “Hispanic Origin” or “N” = “Not of Hispanic Origin” or “U” = “Unknown or Not Reported.” It should be noted that many agencies decline reporting the ethnicity of victims and offenders. (A1).</t>
+  </si>
+  <si>
+    <t>– An alphanumeric variable representing whether the offender was “M”=”Male” or “F”=”Female” or “U” indicating “Unknown” gender, usually in conditions in which the offender had not been identified at the time of the report. (A1).</t>
+  </si>
+  <si>
+    <t>A three-digit numeric variable describing the age in years of the offender. When the offender was not identified at the time of the report, age was reported as 999. A value of 99 represents all offenders 99 or older. (F3.0).</t>
+  </si>
+  <si>
+    <t>– An alphanumeric variable representing whether the offender was “A” = “Asian or Pacific Islander” or “B” = “Black” or “I” = “American Indian or Alaskan Native” or “W” = “White” or “U” = “Unknown” race, usually in conditions in which the offender had not been identified at the time of the report. (A1).</t>
+  </si>
+  <si>
+    <t>– An alphanumeric variable representing whether the offender was “H” = “Hispanic Origin” or “N” = “Not of Hispanic Origin” or “U” = “Unknown or Not Reported.” It should be noted that many agencies decline reporting the ethnicity of victims and offenders. (A1).</t>
+  </si>
+  <si>
+    <t>– A two-digit numeric variable representing the weapon used in the crime. (F2.0).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An alphanumeric variable describing the relationship between the victim and the offender, if any. </t>
+  </si>
+  <si>
+    <t>The number of additional victims (not counting the victim included in the current record) included in the Supplementary Homicide Report’s incident record, which can accept up to 10 additional victims in a single incident report. (F3.0) Incidents of mass murder of more than 11 victims would require multiple SHR incident reports. The Murder Accountability Project’s database captures all reported homicide victims as separate cases. Associated victims will have identical ID numbers</t>
+  </si>
+  <si>
+    <t>The number of additional offenders (not counting the offender included in the current record) included in the Supplementary Homicide Report’s incident record, which can accept up to 10 additional offenders in a single incident report. (F3.0) Unlike victims, the Murder Accountability Project does not create multiple case reports for additional offenders. Only the first offender listed in the original SHR report is included.</t>
+  </si>
+  <si>
+    <t>An eight-digit numeric variable representing the Census Bureau’s Federal Information Processing Standards (FIPS) code for the Metropolitan Statistical Area from which a record was reported. When using the Comma Separated Values format file (file extension=.csv) the original FIPS coding is replaced with the label indicating the metropolitan area. (F8.0).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The month of homicide occurrence or when the victim’s body was recovered. </t>
+  </si>
+  <si>
+    <t>MAP-generated identifier if record provided by FBI (SOURCE=1) or was obtained by MAP under the Freedom of Information Act from an Agency not participating in SHR reporting to the FBI (SOURCE=0). Numeric single digit format. (F1.0).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,10 +227,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -161,6 +241,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -207,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,9 +327,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -273,6 +379,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -448,14 +572,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,196 +589,268 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="C9" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
+      </c>
+      <c r="C25" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
begin cleaning final submission
</commit_message>
<xml_diff>
--- a/Lab 1/Data/data_description.xlsx
+++ b/Lab 1/Data/data_description.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Walt\Desktop\datascience\7331\ML1-Visualization-and-Data-Preprocessing-jamie_proj1\ML1-Visualization-and-Data-Preprocessing-jamie_proj1\Lab 1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prettyvo/Documents/Education/Graduate_school/semesters/2020 Autumn/Machine Learning I/Projects/Clean2_9_6_2020/ML1-Visualization-and-Data-Preprocessing/Lab 1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E49605-25CF-9146-B6D6-4D5FFDE9855F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,82 +100,82 @@
     <t>Record Source</t>
   </si>
   <si>
-    <t>Unique record identifier generated by MAP based upon the YEAR, MONTH, INCIDENT and ORI code in the report. Alphanumeric 16-character format (A16).</t>
-  </si>
-  <si>
-    <t>The alphanumeric variable describing the name of the law enforcement agency making the report. (A450).</t>
-  </si>
-  <si>
-    <t>– The one-digit numeric code describing the type of law enforcement agency making the report so that 1=Sheriff, 2=County Police, 3=Municipality, 5=Primary State Law Enforcement usually meaning the State Police, 6=Special Police, 7=Constable, 8=Tribal Police, 9=Regional Police. When using the Comma Separated Values format file (file extension=.csv) the original FBI numbering scheme is replaced with the alphanumeric label. (F1.0).</t>
-  </si>
-  <si>
-    <t>Alphanumeric variable describing the original FBI naming and abbreviating scheme for the state of the reporting agency. (A6).</t>
-  </si>
-  <si>
-    <t>The one-digit numeric code describing the type of law enforcement agency making the report so that 1=Sheriff, 2=County Police, 3=Municipality, 5=Primary State Law Enforcement usually meaning the State Police, 6=Special Police, 7=Constable, 8=Tribal Police, 9=Regional Police. When using the Comma Separated Values format file (file extension=.csv) the original FBI numbering scheme is replaced with the alphanumeric label. (F1.0).</t>
-  </si>
-  <si>
     <t>Year of homicide (or when victim’s body was recovered.) Numeric four digit. (F4.0).</t>
   </si>
   <si>
-    <t>– A three-digit number describing the case number within the month in which a homicide occurred. This does not necessarily correspond to the actual case number used inhouse by police agencies. It is used to assist in building a unique record number for each case and to differentiate each case reported within the same month. (F3.0)</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable defining whether the report was “A” = “Murder or Nonnegligent manslaughter” or “B” = “Manslaughter by Negligence.” (A1).</t>
-  </si>
-  <si>
-    <t>MAP-generated indicator whether Offender was identified at time report was made (SOLVED=1) or not identified (SOLVED=0). Numeric single digit format. (F1.0).</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable representing whether the victim was “M” = ”Male” or “F” = ”Female” or “U” indicating “Unknown” gender, usually for conditions in which incomplete remains were recovered. (A1).</t>
-  </si>
-  <si>
-    <t>A three-digit numeric variable describing the age in years of the victim. To allow for simpler mathematical calculations, MAP has changed the original alphanumeric coding of “NB” for new born and “BB” for infant to a numeric value of zero to indicate the victim had not achieved a full year of life. A value of 99, as in the original numbering scheme, represents all victims 99 or older. A value of 999 represents victims whose age was not reported, usually because the victim was unidentified and the age was unknown. (F3.0).</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable representing whether the victim was “A” = “Asian or Pacific Islander” or “B” = “Black” or “I” = “American Indian or Alaskan Native” or “W” = “White” or “U” victim was of “Unknown” race. (A1).</t>
-  </si>
-  <si>
-    <t>An alphanumeric variable representing whether the victim was “H” = “Hispanic Origin” or “N” = “Not of Hispanic Origin” or “U” = “Unknown or Not Reported.” It should be noted that many agencies decline reporting the ethnicity of victims and offenders. (A1).</t>
-  </si>
-  <si>
-    <t>– An alphanumeric variable representing whether the offender was “M”=”Male” or “F”=”Female” or “U” indicating “Unknown” gender, usually in conditions in which the offender had not been identified at the time of the report. (A1).</t>
-  </si>
-  <si>
-    <t>A three-digit numeric variable describing the age in years of the offender. When the offender was not identified at the time of the report, age was reported as 999. A value of 99 represents all offenders 99 or older. (F3.0).</t>
-  </si>
-  <si>
-    <t>– An alphanumeric variable representing whether the offender was “A” = “Asian or Pacific Islander” or “B” = “Black” or “I” = “American Indian or Alaskan Native” or “W” = “White” or “U” = “Unknown” race, usually in conditions in which the offender had not been identified at the time of the report. (A1).</t>
-  </si>
-  <si>
-    <t>– An alphanumeric variable representing whether the offender was “H” = “Hispanic Origin” or “N” = “Not of Hispanic Origin” or “U” = “Unknown or Not Reported.” It should be noted that many agencies decline reporting the ethnicity of victims and offenders. (A1).</t>
-  </si>
-  <si>
-    <t>– A two-digit numeric variable representing the weapon used in the crime. (F2.0).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An alphanumeric variable describing the relationship between the victim and the offender, if any. </t>
-  </si>
-  <si>
     <t>The number of additional victims (not counting the victim included in the current record) included in the Supplementary Homicide Report’s incident record, which can accept up to 10 additional victims in a single incident report. (F3.0) Incidents of mass murder of more than 11 victims would require multiple SHR incident reports. The Murder Accountability Project’s database captures all reported homicide victims as separate cases. Associated victims will have identical ID numbers</t>
   </si>
   <si>
     <t>The number of additional offenders (not counting the offender included in the current record) included in the Supplementary Homicide Report’s incident record, which can accept up to 10 additional offenders in a single incident report. (F3.0) Unlike victims, the Murder Accountability Project does not create multiple case reports for additional offenders. Only the first offender listed in the original SHR report is included.</t>
   </si>
   <si>
-    <t>An eight-digit numeric variable representing the Census Bureau’s Federal Information Processing Standards (FIPS) code for the Metropolitan Statistical Area from which a record was reported. When using the Comma Separated Values format file (file extension=.csv) the original FIPS coding is replaced with the label indicating the metropolitan area. (F8.0).</t>
-  </si>
-  <si>
     <t xml:space="preserve">The month of homicide occurrence or when the victim’s body was recovered. </t>
   </si>
   <si>
-    <t>MAP-generated identifier if record provided by FBI (SOURCE=1) or was obtained by MAP under the Freedom of Information Act from an Agency not participating in SHR reporting to the FBI (SOURCE=0). Numeric single digit format. (F1.0).</t>
+    <t>Unique record identifier generated by MAP based upon the YEAR, MONTH, INCIDENT and ORI code in the report.</t>
+  </si>
+  <si>
+    <t>The alphanumeric variable describing the name of the law enforcement agency making the report.</t>
+  </si>
+  <si>
+    <t>Unique Agency identifier.</t>
+  </si>
+  <si>
+    <t>The type of law enforcement agency making the report. (e.g. Sheriff)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphanumeric variable describing the original FBI naming and abbreviating scheme for the city of the reporting agency. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alphanumeric variable describing the original FBI naming and abbreviating scheme for the state of the reporting agency. </t>
+  </si>
+  <si>
+    <t>A three-digit number describing the case number within the month in which a homicide occurred.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAP-generated indicator whether Offender was identified at time report was made (SOLVED=1) or not identified (SOLVED=0). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">An alphanumeric variable defining whether the report was "Murder or Nonnegligent manslaughter” or “Manslaughter by Negligence.” </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable describing the age in years of the victim. A value of 0 indicates the victim had not achieved a full year of life, 99 represents all victims 99 or older, and 998 represents victims whose age was not reported, usually because the victim was unidentified and the age was unknown. </t>
+  </si>
+  <si>
+    <t>Variable representing whether the victim's race</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable representing whether the victim was  ”Male”, ”Female” or  “Unknown” gender, usually for conditions in which incomplete remains were recovered. </t>
+  </si>
+  <si>
+    <t>Variable representing whether the victim was “Hispanic Origin”, “Not of Hispanic Origin” or “Unknown or Not Reported.” Many agencies declined reporting the ethnicity of victims and offenders.</t>
+  </si>
+  <si>
+    <t>Variable representing whether the offender was”Male”, ”Female” or “Unknown” gender, usually in conditions in which the offender had not been identified at the time of the report.</t>
+  </si>
+  <si>
+    <t>Variable describing the age in years of the offender. When the offender was not identified at the time of the report, age was reported as 999. A value of 99 represents all offenders 99 or older.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable representing whether the offender's race, "unkown" usually in conditions in which the offender had not been identified at the time of the report. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable representing whether the offender was “Hispanic Origin”, “Not of Hispanic Origin” or“Unknown or Not Reported.” Many agencies declined reporting the ethnicity of victims and offenders. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable describing the relationship between the victim and the offender, if any. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Variable representing the weapon used in the crime. </t>
+  </si>
+  <si>
+    <t>MAP-generated identifier if record provided by FBI or was obtained by MAP under the Freedom of Information Act from an Agency not participating in SHR reporting to the FBI.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,14 +228,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,284 +574,216 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="142.33203125" style="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="24" spans="1:2" ht="48" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="210" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
+    <row r="25" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C25" t="s">
+      <c r="B25" s="1" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>